<commit_message>
selesai vr1 eps no
</commit_message>
<xml_diff>
--- a/analisis/hasil analisis.xlsx
+++ b/analisis/hasil analisis.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rama Nitip\python\snake-game-ai\analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8017AD0D-A732-49AF-8A53-3DF0ACFA11EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4076766F-F596-4509-BF44-8D689B06F462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Game high score</t>
   </si>
@@ -36,11 +36,17 @@
   <si>
     <t>Visual Range</t>
   </si>
+  <si>
+    <t>32.0m 6.95s</t>
+  </si>
+  <si>
+    <t>waktu sampai 500 games</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -568,17 +574,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -934,11 +940,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="D3:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,10 +953,10 @@
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
@@ -963,114 +969,137 @@
       <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D4" s="4">
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D5" s="5"/>
-      <c r="E5" s="7">
-        <v>0.01</v>
+      <c r="F4" s="2">
+        <v>42</v>
+      </c>
+      <c r="G4" s="2">
+        <v>359</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="7"/>
+      <c r="E5" s="5">
+        <v>0.02</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="4">
-        <v>5</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="5"/>
-      <c r="E7" s="7">
-        <v>0.01</v>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="7"/>
+      <c r="E7" s="5">
+        <v>0.02</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="4">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="6">
         <v>9</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="5"/>
-      <c r="E9" s="7">
-        <v>0.01</v>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="7"/>
+      <c r="E9" s="5">
+        <v>0.02</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="4">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="6">
         <v>21</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="5"/>
-      <c r="E11" s="7">
-        <v>0.01</v>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="7"/>
+      <c r="E11" s="5">
+        <v>0.02</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
selesai vr3 eps no
</commit_message>
<xml_diff>
--- a/analisis/hasil analisis.xlsx
+++ b/analisis/hasil analisis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rama Nitip\python\snake-game-ai\analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4076766F-F596-4509-BF44-8D689B06F462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC07304-8085-463E-8160-75E6091038EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Game high score</t>
   </si>
@@ -37,10 +37,13 @@
     <t>Visual Range</t>
   </si>
   <si>
-    <t>32.0m 6.95s</t>
+    <t>waktu sampai 500 games</t>
   </si>
   <si>
-    <t>waktu sampai 500 games</t>
+    <t>32m 6.95s</t>
+  </si>
+  <si>
+    <t>50m 12.97s</t>
   </si>
 </sst>
 </file>
@@ -944,7 +947,7 @@
   <dimension ref="D3:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,7 +973,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="4:8" x14ac:dyDescent="0.25">
@@ -987,7 +990,7 @@
         <v>359</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="4:8" x14ac:dyDescent="0.25">
@@ -1006,9 +1009,15 @@
       <c r="E6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="F6" s="2">
+        <v>77</v>
+      </c>
+      <c r="G6" s="2">
+        <v>225</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D7" s="7"/>

</xml_diff>

<commit_message>
selesai vr3 eps 2
</commit_message>
<xml_diff>
--- a/analisis/hasil analisis.xlsx
+++ b/analisis/hasil analisis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rama Nitip\python\snake-game-ai\analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rama Nitip\python\snake game ai\analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC07304-8085-463E-8160-75E6091038EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D553FD-1A5E-4955-B045-C2DE1E1B968C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Game high score</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>50m 12.97s</t>
+  </si>
+  <si>
+    <t>59m 12.97s</t>
   </si>
 </sst>
 </file>
@@ -947,19 +950,19 @@
   <dimension ref="D3:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:8" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
@@ -976,7 +979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D4" s="6">
         <v>1</v>
       </c>
@@ -993,7 +996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D5" s="7"/>
       <c r="E5" s="5">
         <v>0.02</v>
@@ -1002,7 +1005,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D6" s="6">
         <v>3</v>
       </c>
@@ -1019,16 +1022,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D7" s="7"/>
       <c r="E7" s="5">
         <v>0.02</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="2">
+        <v>72</v>
+      </c>
+      <c r="G7" s="2">
+        <v>227</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D8" s="6">
         <v>9</v>
       </c>
@@ -1039,7 +1048,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D9" s="7"/>
       <c r="E9" s="5">
         <v>0.02</v>
@@ -1048,7 +1057,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D10" s="6">
         <v>21</v>
       </c>
@@ -1059,7 +1068,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D11" s="7"/>
       <c r="E11" s="5">
         <v>0.02</v>
@@ -1068,42 +1077,42 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>

</xml_diff>

<commit_message>
selesai vr 9 eps no,1
</commit_message>
<xml_diff>
--- a/analisis/hasil analisis.xlsx
+++ b/analisis/hasil analisis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rama Nitip\python\snake game ai\analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rama Nitip\python\snake-game-ai\analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D553FD-1A5E-4955-B045-C2DE1E1B968C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE8A959-F3EF-4C56-96D4-74F614334D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Game high score</t>
   </si>
@@ -48,6 +48,12 @@
   <si>
     <t>59m 12.97s</t>
   </si>
+  <si>
+    <t>32m 59.36s</t>
+  </si>
+  <si>
+    <t>19m 57.09s</t>
+  </si>
 </sst>
 </file>
 
@@ -370,7 +376,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -524,6 +530,17 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -571,7 +588,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -590,6 +607,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -947,22 +970,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D3:H17"/>
+  <dimension ref="D3:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:8" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="4:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
@@ -979,7 +1002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D4" s="6">
         <v>1</v>
       </c>
@@ -996,7 +1019,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D5" s="7"/>
       <c r="E5" s="5">
         <v>0.02</v>
@@ -1005,7 +1028,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D6" s="6">
         <v>3</v>
       </c>
@@ -1022,7 +1045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D7" s="7"/>
       <c r="E7" s="5">
         <v>0.02</v>
@@ -1037,94 +1060,120 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D8" s="6">
         <v>9</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D9" s="7"/>
-      <c r="E9" s="5">
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="9"/>
+      <c r="E9" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="F9" s="2">
+        <v>70</v>
+      </c>
+      <c r="G9" s="2">
+        <v>286</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="7"/>
+      <c r="E10" s="5">
         <v>0.02</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D10" s="6">
-        <v>21</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>1</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D11" s="7"/>
-      <c r="E11" s="5">
-        <v>0.02</v>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="6">
+        <v>21</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.35">
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="7"/>
+      <c r="E12" s="5">
+        <v>0.02</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D8:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>